<commit_message>
Add terminal block for ground banana.
</commit_message>
<xml_diff>
--- a/6WLS-40W-BOM.xlsx
+++ b/6WLS-40W-BOM.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>Qty</t>
   </si>
@@ -218,6 +218,18 @@
   </si>
   <si>
     <t>EC7C-12S15</t>
+  </si>
+  <si>
+    <t>MKDSN</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Terminal Block</t>
+  </si>
+  <si>
+    <t>PHOENIX</t>
   </si>
 </sst>
 </file>
@@ -261,9 +273,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,10 +577,10 @@
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -587,7 +605,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -610,7 +628,7 @@
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -656,7 +674,7 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -722,7 +740,7 @@
       <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -748,7 +766,7 @@
       <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -774,7 +792,7 @@
       <c r="G9" t="s">
         <v>53</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -800,8 +818,34 @@
       <c r="G10" t="s">
         <v>51</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1729128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>